<commit_message>
Slight cleanup of Ground_Truth_Topics.xlsx
</commit_message>
<xml_diff>
--- a/topic-files/Ground_Truth_Topics.xlsx
+++ b/topic-files/Ground_Truth_Topics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktuoh\Documents\School\MCS-DS\CS_410_Text_Info_Systems\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktuoh\Documents\School\MCS-DS\CS_410_Text_Info_Systems\Project\CourseProject\topic-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B88DE8-0724-41FE-9737-6C6347BCE864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7353AE7-32EF-45A5-B97B-E98DF54A76CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35930" yWindow="190" windowWidth="21270" windowHeight="21160" activeTab="2" xr2:uid="{0F37B134-5501-4313-8724-3C793E42205F}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -213,9 +213,6 @@
     <t>https://github.com/hernang2/CourseProject</t>
   </si>
   <si>
-    <t>Extend ExpertSearch system</t>
-  </si>
-  <si>
     <t>Crawl faculty webpages, harvest top terms from bios</t>
   </si>
   <si>
@@ -364,6 +361,9 @@
   </si>
   <si>
     <t>Based on the sample of projects and "ground truth" topics in the Selected Project Topics tab.</t>
+  </si>
+  <si>
+    <t>Causal topic mining</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kurt Tuohy" refreshedDate="44513.70072291667" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="61" xr:uid="{92DFCEC7-18E8-45E9-9927-46E16BD049B4}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kurt Tuohy" refreshedDate="44513.863050810185" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="61" xr:uid="{92DFCEC7-18E8-45E9-9927-46E16BD049B4}">
   <cacheSource type="worksheet">
     <worksheetSource name="Selected_Project_Topic_Table"/>
   </cacheSource>
@@ -470,7 +470,7 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Topics" numFmtId="0">
-      <sharedItems count="43">
+      <sharedItems count="44">
         <s v="Never started"/>
         <s v="Detect offensive language"/>
         <s v="Sentiment analysis"/>
@@ -489,9 +489,9 @@
         <s v="Quality of life sentiment analysis for US states from Twitter"/>
         <s v="Rate sentiment for quality of life dimensions by US state"/>
         <s v="Topic mining"/>
+        <s v="Causal topic mining"/>
         <s v="Topic modeling with time series feedback"/>
         <s v="System extension"/>
-        <s v="Extend ExpertSearch system"/>
         <s v="ExpertSearch"/>
         <s v="Crawl faculty webpages, harvest top terms from bios"/>
         <s v="EducationalWeb"/>
@@ -512,6 +512,7 @@
         <s v="Make MetaPy compatible with Python 3.8"/>
         <s v="Retrieve and search top tech companies"/>
         <s v="Mining causal topics" u="1"/>
+        <s v="Extend ExpertSearch system" u="1"/>
         <s v="Extend EducationalWeb" u="1"/>
         <s v="Replicate ExpertSearch system" u="1"/>
       </sharedItems>
@@ -651,7 +652,7 @@
     <m/>
   </r>
   <r>
-    <s v="https://github.com/hernang2/CourseProject"/>
+    <s v="https://github.com/Ludy11xc/CS-410-CourseProject"/>
     <x v="19"/>
     <m/>
   </r>
@@ -672,7 +673,7 @@
   </r>
   <r>
     <s v="https://github.com/henryg3/CourseProject"/>
-    <x v="19"/>
+    <x v="20"/>
     <m/>
   </r>
   <r>
@@ -707,7 +708,7 @@
   </r>
   <r>
     <s v="https://github.com/tgw4uiuc/CourseProject"/>
-    <x v="19"/>
+    <x v="20"/>
     <m/>
   </r>
   <r>
@@ -747,7 +748,7 @@
   </r>
   <r>
     <s v="https://github.com/Asciotti/CourseProject"/>
-    <x v="19"/>
+    <x v="20"/>
     <m/>
   </r>
   <r>
@@ -767,7 +768,7 @@
   </r>
   <r>
     <s v="https://github.com/xiang-wang2020/CourseProject"/>
-    <x v="19"/>
+    <x v="20"/>
     <m/>
   </r>
   <r>
@@ -839,12 +840,12 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EF331B7-9265-4CE7-B555-BF50478D5EA0}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EF331B7-9265-4CE7-B555-BF50478D5EA0}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A5:B46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="44">
+      <items count="45">
         <item x="30"/>
         <item x="36"/>
         <item x="12"/>
@@ -854,8 +855,8 @@
         <item x="8"/>
         <item x="1"/>
         <item x="9"/>
+        <item m="1" x="42"/>
         <item m="1" x="41"/>
-        <item x="20"/>
         <item x="26"/>
         <item x="24"/>
         <item x="33"/>
@@ -869,25 +870,26 @@
         <item x="25"/>
         <item x="15"/>
         <item x="16"/>
-        <item m="1" x="42"/>
+        <item m="1" x="43"/>
         <item x="5"/>
         <item x="39"/>
         <item x="14"/>
         <item x="2"/>
         <item x="29"/>
         <item x="3"/>
-        <item x="19"/>
+        <item x="20"/>
         <item x="37"/>
         <item x="4"/>
         <item x="13"/>
         <item x="32"/>
-        <item x="18"/>
+        <item x="19"/>
         <item x="34"/>
         <item x="28"/>
         <item x="17"/>
         <item x="21"/>
         <item x="23"/>
         <item x="27"/>
+        <item x="18"/>
         <item t="default"/>
       </items>
       <autoSortScope>
@@ -922,109 +924,109 @@
       <x v="25"/>
     </i>
     <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
       <x v="40"/>
     </i>
     <i>
-      <x v="8"/>
-    </i>
-    <i>
       <x v="42"/>
     </i>
     <i>
-      <x v="41"/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="16"/>
     </i>
     <i>
       <x v="27"/>
     </i>
     <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
       <x v="35"/>
     </i>
     <i>
-      <x v="6"/>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="3"/>
     </i>
     <i>
       <x v="11"/>
     </i>
     <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
       <x v="26"/>
     </i>
     <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="36"/>
+      <x v="21"/>
+    </i>
+    <i>
+      <x/>
     </i>
     <i>
       <x v="22"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="21"/>
     </i>
     <i t="grand">
       <x/>
@@ -1393,7 +1395,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1407,7 +1409,7 @@
   <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,7 +1617,7 @@
         <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1623,15 +1625,15 @@
         <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1639,7 +1641,7 @@
         <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1647,7 +1649,7 @@
         <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1655,12 +1657,12 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
         <v>39</v>
@@ -1668,42 +1670,42 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
         <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
         <v>61</v>
-      </c>
-      <c r="B34" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
         <v>42</v>
@@ -1711,15 +1713,15 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
         <v>63</v>
-      </c>
-      <c r="B36" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
@@ -1727,23 +1729,23 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -1751,39 +1753,39 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" t="s">
         <v>71</v>
-      </c>
-      <c r="B43" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" t="s">
         <v>76</v>
-      </c>
-      <c r="B44" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45" t="s">
         <v>39</v>
@@ -1791,23 +1793,23 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -1815,7 +1817,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" t="s">
         <v>39</v>
@@ -1823,15 +1825,15 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
@@ -1839,42 +1841,42 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" t="s">
         <v>79</v>
-      </c>
-      <c r="B52" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
@@ -1882,42 +1884,42 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B57" t="s">
         <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" t="s">
         <v>89</v>
-      </c>
-      <c r="B60" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B61" t="s">
         <v>49</v>
@@ -1925,10 +1927,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" t="s">
         <v>91</v>
-      </c>
-      <c r="B62" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1942,7 +1944,7 @@
     <hyperlink ref="A17" r:id="rId7" xr:uid="{840D71FB-93D2-48DE-BEF3-904434C7792D}"/>
     <hyperlink ref="A20" r:id="rId8" xr:uid="{B1FF0D70-0D66-44A1-BD21-1CD3F42F42B0}"/>
     <hyperlink ref="A23" r:id="rId9" xr:uid="{5FDE10F4-C0C1-4D43-B273-B36306CB65A2}"/>
-    <hyperlink ref="A26" r:id="rId10" xr:uid="{CE461E31-E678-4C76-848F-F6DD3C621E25}"/>
+    <hyperlink ref="A27" r:id="rId10" xr:uid="{CE461E31-E678-4C76-848F-F6DD3C621E25}"/>
     <hyperlink ref="A30" r:id="rId11" xr:uid="{9BB82FE0-4CF4-4787-91C3-E0702F000D02}"/>
     <hyperlink ref="A33" r:id="rId12" xr:uid="{30B6A3DB-3A47-4522-83F3-B57566633331}"/>
     <hyperlink ref="A35" r:id="rId13" xr:uid="{239AE7BF-BF0E-4BCC-BE19-B22B92FD6A4E}"/>
@@ -1963,33 +1965,33 @@
     <hyperlink ref="A21" r:id="rId28" xr:uid="{158D91D6-37FF-4D16-87AE-CBFECFB1872E}"/>
     <hyperlink ref="A22" r:id="rId29" xr:uid="{4153AD43-AF0F-42BD-9679-AE9EE623EE82}"/>
     <hyperlink ref="A24" r:id="rId30" xr:uid="{F3714B50-D988-4E82-970B-A860A5983F67}"/>
-    <hyperlink ref="A25" r:id="rId31" xr:uid="{1CF17632-8764-418E-A9F9-AF14C4E44611}"/>
-    <hyperlink ref="A27" r:id="rId32" xr:uid="{FF10D34C-05B4-421F-802A-1CAB0EA55FD8}"/>
-    <hyperlink ref="A29" r:id="rId33" xr:uid="{07FC7BAD-20FC-47BB-8751-EE85C03E1A6C}"/>
-    <hyperlink ref="A31" r:id="rId34" xr:uid="{D2480FBC-E5B1-4382-911E-B87C41FACF9D}"/>
-    <hyperlink ref="A32" r:id="rId35" xr:uid="{E68D708E-94F6-4DB3-B61B-DB5DEF749AB4}"/>
-    <hyperlink ref="A34" r:id="rId36" xr:uid="{89BDA958-FCA2-4D0F-BAD3-4F097AAD5559}"/>
-    <hyperlink ref="A36" r:id="rId37" xr:uid="{2233BD9D-5DE3-4B50-B026-459DB7B2B7FE}"/>
-    <hyperlink ref="A39" r:id="rId38" xr:uid="{11D93E4B-3E7C-43D8-A360-6358AB5775EE}"/>
-    <hyperlink ref="A41" r:id="rId39" xr:uid="{49CEFA82-CEBC-4E5F-ADAB-1370E507E76D}"/>
-    <hyperlink ref="A42" r:id="rId40" xr:uid="{9FCF0046-F3F3-47FE-A049-2BA17E108B00}"/>
-    <hyperlink ref="A43" r:id="rId41" xr:uid="{5A9F00D8-D2F9-4A28-9D4E-6816B816166E}"/>
-    <hyperlink ref="A45" r:id="rId42" xr:uid="{4B52E770-79B8-4200-B061-540B6DBB5373}"/>
-    <hyperlink ref="A46" r:id="rId43" xr:uid="{3D7CD35F-E83C-4F19-A93A-0F2E79024AE5}"/>
-    <hyperlink ref="A47" r:id="rId44" xr:uid="{09341998-B55F-4604-969D-FA2C4785D63E}"/>
-    <hyperlink ref="A48" r:id="rId45" xr:uid="{AC004112-2A44-4BE7-ADAE-D7F46FDFACFA}"/>
-    <hyperlink ref="A50" r:id="rId46" xr:uid="{ACCB3ACF-6972-4B9B-B527-B9A357F86030}"/>
-    <hyperlink ref="A51" r:id="rId47" xr:uid="{F5FBB7A5-B2BE-4299-9BBE-10356966EE8E}"/>
-    <hyperlink ref="A52" r:id="rId48" xr:uid="{8B9A38ED-361D-4FEE-A522-7AD6650C7153}"/>
-    <hyperlink ref="A54" r:id="rId49" xr:uid="{C6402A08-A987-4321-9CA3-A2B6F35EDE4D}"/>
-    <hyperlink ref="A55" r:id="rId50" xr:uid="{A8EE9331-3E78-4FBB-ACA7-01D91A5A9A2E}"/>
-    <hyperlink ref="A56" r:id="rId51" xr:uid="{21527383-4191-472B-B2B4-CB8F68F4FB17}"/>
-    <hyperlink ref="A60" r:id="rId52" xr:uid="{819C5A54-92D6-4730-92C9-EB8DEEF52E7F}"/>
-    <hyperlink ref="A61" r:id="rId53" xr:uid="{6C70B721-ED03-4D9C-ACF6-A301A3A7BF27}"/>
-    <hyperlink ref="A62" r:id="rId54" xr:uid="{E9BF18D2-A036-41EC-8A36-983569B28D36}"/>
-    <hyperlink ref="A38" r:id="rId55" xr:uid="{2A8A873F-71B3-47FA-8211-4D17375AEE46}"/>
-    <hyperlink ref="A28" r:id="rId56" xr:uid="{A70112D7-FAEE-4C6F-A717-E00144C96993}"/>
-    <hyperlink ref="A59" r:id="rId57" xr:uid="{63E22808-BB28-459D-B964-E6B20444BCF4}"/>
+    <hyperlink ref="A26" r:id="rId31" xr:uid="{1CF17632-8764-418E-A9F9-AF14C4E44611}"/>
+    <hyperlink ref="A29" r:id="rId32" xr:uid="{07FC7BAD-20FC-47BB-8751-EE85C03E1A6C}"/>
+    <hyperlink ref="A31" r:id="rId33" xr:uid="{D2480FBC-E5B1-4382-911E-B87C41FACF9D}"/>
+    <hyperlink ref="A32" r:id="rId34" xr:uid="{E68D708E-94F6-4DB3-B61B-DB5DEF749AB4}"/>
+    <hyperlink ref="A34" r:id="rId35" xr:uid="{89BDA958-FCA2-4D0F-BAD3-4F097AAD5559}"/>
+    <hyperlink ref="A36" r:id="rId36" xr:uid="{2233BD9D-5DE3-4B50-B026-459DB7B2B7FE}"/>
+    <hyperlink ref="A39" r:id="rId37" xr:uid="{11D93E4B-3E7C-43D8-A360-6358AB5775EE}"/>
+    <hyperlink ref="A41" r:id="rId38" xr:uid="{49CEFA82-CEBC-4E5F-ADAB-1370E507E76D}"/>
+    <hyperlink ref="A42" r:id="rId39" xr:uid="{9FCF0046-F3F3-47FE-A049-2BA17E108B00}"/>
+    <hyperlink ref="A43" r:id="rId40" xr:uid="{5A9F00D8-D2F9-4A28-9D4E-6816B816166E}"/>
+    <hyperlink ref="A45" r:id="rId41" xr:uid="{4B52E770-79B8-4200-B061-540B6DBB5373}"/>
+    <hyperlink ref="A46" r:id="rId42" xr:uid="{3D7CD35F-E83C-4F19-A93A-0F2E79024AE5}"/>
+    <hyperlink ref="A47" r:id="rId43" xr:uid="{09341998-B55F-4604-969D-FA2C4785D63E}"/>
+    <hyperlink ref="A48" r:id="rId44" xr:uid="{AC004112-2A44-4BE7-ADAE-D7F46FDFACFA}"/>
+    <hyperlink ref="A50" r:id="rId45" xr:uid="{ACCB3ACF-6972-4B9B-B527-B9A357F86030}"/>
+    <hyperlink ref="A51" r:id="rId46" xr:uid="{F5FBB7A5-B2BE-4299-9BBE-10356966EE8E}"/>
+    <hyperlink ref="A52" r:id="rId47" xr:uid="{8B9A38ED-361D-4FEE-A522-7AD6650C7153}"/>
+    <hyperlink ref="A54" r:id="rId48" xr:uid="{C6402A08-A987-4321-9CA3-A2B6F35EDE4D}"/>
+    <hyperlink ref="A55" r:id="rId49" xr:uid="{A8EE9331-3E78-4FBB-ACA7-01D91A5A9A2E}"/>
+    <hyperlink ref="A56" r:id="rId50" xr:uid="{21527383-4191-472B-B2B4-CB8F68F4FB17}"/>
+    <hyperlink ref="A60" r:id="rId51" xr:uid="{819C5A54-92D6-4730-92C9-EB8DEEF52E7F}"/>
+    <hyperlink ref="A61" r:id="rId52" xr:uid="{6C70B721-ED03-4D9C-ACF6-A301A3A7BF27}"/>
+    <hyperlink ref="A62" r:id="rId53" xr:uid="{E9BF18D2-A036-41EC-8A36-983569B28D36}"/>
+    <hyperlink ref="A38" r:id="rId54" xr:uid="{2A8A873F-71B3-47FA-8211-4D17375AEE46}"/>
+    <hyperlink ref="A28" r:id="rId55" xr:uid="{A70112D7-FAEE-4C6F-A717-E00144C96993}"/>
+    <hyperlink ref="A59" r:id="rId56" xr:uid="{63E22808-BB28-459D-B964-E6B20444BCF4}"/>
+    <hyperlink ref="A25" r:id="rId57" xr:uid="{3D51EB8D-3269-4822-A7EC-DE976FD23CF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2014,12 +2016,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2027,7 +2029,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2088,7 +2090,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B13" s="5">
         <v>2</v>
@@ -2096,7 +2098,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B14" s="5">
         <v>2</v>
@@ -2104,7 +2106,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -2112,7 +2114,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="B16" s="5">
         <v>1</v>
@@ -2120,7 +2122,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
@@ -2128,7 +2130,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
@@ -2136,7 +2138,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
@@ -2144,7 +2146,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -2152,7 +2154,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
@@ -2160,7 +2162,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="B22" s="5">
         <v>1</v>
@@ -2176,7 +2178,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
@@ -2184,7 +2186,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
@@ -2192,7 +2194,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
@@ -2200,7 +2202,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="B27" s="5">
         <v>1</v>
@@ -2208,7 +2210,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B28" s="5">
         <v>1</v>
@@ -2216,7 +2218,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
@@ -2224,7 +2226,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B30" s="5">
         <v>1</v>
@@ -2232,7 +2234,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B31" s="5">
         <v>1</v>
@@ -2240,7 +2242,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="B32" s="5">
         <v>1</v>
@@ -2248,7 +2250,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="B33" s="5">
         <v>1</v>
@@ -2264,7 +2266,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="B35" s="5">
         <v>1</v>
@@ -2272,7 +2274,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="B36" s="5">
         <v>1</v>
@@ -2280,7 +2282,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B37" s="5">
         <v>1</v>
@@ -2288,7 +2290,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B38" s="5">
         <v>1</v>
@@ -2296,7 +2298,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B39" s="5">
         <v>1</v>
@@ -2304,7 +2306,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B40" s="5">
         <v>1</v>
@@ -2312,7 +2314,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B41" s="5">
         <v>1</v>
@@ -2320,7 +2322,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B42" s="5">
         <v>1</v>
@@ -2328,7 +2330,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
@@ -2336,7 +2338,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
@@ -2344,7 +2346,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B45" s="5">
         <v>1</v>
@@ -2352,7 +2354,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" s="5">
         <v>61</v>
@@ -2379,12 +2381,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2405,7 +2407,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2423,15 +2425,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2507,43 +2509,43 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
         <v>100</v>
-      </c>
-      <c r="B28" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating 'ground truth' document. Drafting document to compare discovered topics and tags with the 'ground truth' topics for sample CS 410 projects.
</commit_message>
<xml_diff>
--- a/topic-files/Ground_Truth_Topics.xlsx
+++ b/topic-files/Ground_Truth_Topics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktuoh\Documents\School\MCS-DS\CS_410_Text_Info_Systems\Project\CourseProject\topic-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFC79E9-E5E7-4E09-9400-20ECB2C29DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C633D58-7D1A-4A0F-A951-483CD68C8B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22030" yWindow="2350" windowWidth="25710" windowHeight="18160" activeTab="1" xr2:uid="{0F37B134-5501-4313-8724-3C793E42205F}"/>
+    <workbookView xWindow="19370" yWindow="3670" windowWidth="23600" windowHeight="18160" activeTab="1" xr2:uid="{0F37B134-5501-4313-8724-3C793E42205F}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="144">
   <si>
     <t>Project Link</t>
   </si>
@@ -338,9 +338,6 @@
     <t>Free topic</t>
   </si>
   <si>
-    <t>Causal topic mining</t>
-  </si>
-  <si>
     <t>High-Level Topic</t>
   </si>
   <si>
@@ -354,6 +351,123 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>https://github.com/Diegoma89/CS410_CourseProject_DM</t>
+  </si>
+  <si>
+    <t>https://github.com/BillyZhaohengLi/PLSAprior</t>
+  </si>
+  <si>
+    <t>MetaPy</t>
+  </si>
+  <si>
+    <t>PLSA with Priors</t>
+  </si>
+  <si>
+    <t>Add function for PLSA with background model and priors to MetaPy</t>
+  </si>
+  <si>
+    <t>Topic mining</t>
+  </si>
+  <si>
+    <t>https://github.com/ElizWang/CourseProject</t>
+  </si>
+  <si>
+    <t>Generate semantic annotations</t>
+  </si>
+  <si>
+    <t>Frequent patterns</t>
+  </si>
+  <si>
+    <t>Context analysis</t>
+  </si>
+  <si>
+    <t>https://github.com/Xinyihe123/LARA</t>
+  </si>
+  <si>
+    <t>https://github.com/adeetikaushal/CourseProject</t>
+  </si>
+  <si>
+    <t>Recommendation systems</t>
+  </si>
+  <si>
+    <t>Book recommendation system</t>
+  </si>
+  <si>
+    <t>https://github.com/amyth18/CourseProject</t>
+  </si>
+  <si>
+    <t>https://github.com/darrenmuliawan/CourseProject</t>
+  </si>
+  <si>
+    <t>Organize email inbox</t>
+  </si>
+  <si>
+    <t>Update ExpertSearch's dataset with new faculty</t>
+  </si>
+  <si>
+    <t>Data collection</t>
+  </si>
+  <si>
+    <t>https://github.com/dattatreya303/CourseProject</t>
+  </si>
+  <si>
+    <t>Generate summaries of podcast transcription</t>
+  </si>
+  <si>
+    <t>Condense transcription</t>
+  </si>
+  <si>
+    <t>https://github.com/devinsburke/CourseProject</t>
+  </si>
+  <si>
+    <t>Condense webpage text</t>
+  </si>
+  <si>
+    <t>https://github.com/diane630/CourseProject</t>
+  </si>
+  <si>
+    <t>Search engine</t>
+  </si>
+  <si>
+    <t>Search book/movie adaptations</t>
+  </si>
+  <si>
+    <t>https://github.com/kikibean/CourseProject</t>
+  </si>
+  <si>
+    <t>Sentiment analysis in financial reports</t>
+  </si>
+  <si>
+    <t>Stock analysis</t>
+  </si>
+  <si>
+    <t>https://github.com/naviCh/CourseProject</t>
+  </si>
+  <si>
+    <t>Dataset creation</t>
+  </si>
+  <si>
+    <t>Collect data and perform sentiment analysis on news-related subreddits</t>
+  </si>
+  <si>
+    <t>https://github.com/pritomsaha/CourseProject</t>
+  </si>
+  <si>
+    <t>Causal topic modeling</t>
+  </si>
+  <si>
+    <t>Time series</t>
+  </si>
+  <si>
+    <t>Contextual text mining using election news and betting market behavior + stock prices</t>
+  </si>
+  <si>
+    <t>https://github.com/sitajothi/CourseProject</t>
+  </si>
+  <si>
+    <t>Analyze stock sentiment from Twitter</t>
   </si>
 </sst>
 </file>
@@ -449,8 +563,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{211A4259-A08B-4C0C-A237-5C41C49A6EC2}" name="Selected_Project_Topic_Table4" displayName="Selected_Project_Topic_Table4" ref="A1:E34" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E34" xr:uid="{612C9047-1189-4A6B-B897-EB8BF18B9FF9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{211A4259-A08B-4C0C-A237-5C41C49A6EC2}" name="Selected_Project_Topic_Table4" displayName="Selected_Project_Topic_Table4" ref="A1:E43" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E43" xr:uid="{612C9047-1189-4A6B-B897-EB8BF18B9FF9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{6A14DB56-DD12-401C-9F31-AB678A85BC28}" name="Project Link"/>
     <tableColumn id="2" xr3:uid="{67882653-FA50-478E-913F-6E9070B41516}" name="High-Level Topic"/>
@@ -463,7 +577,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{463CC7ED-5444-42DB-8069-1A990E370B56}" name="Table2" displayName="Table2" ref="A4:B30" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{463CC7ED-5444-42DB-8069-1A990E370B56}" name="Table2" displayName="Table2" ref="A4:B30" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A4:B30" xr:uid="{463CC7ED-5444-42DB-8069-1A990E370B56}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4E376CD6-347D-4CF2-BC1F-CBA09F90B6A3}" name="Topic"/>
@@ -806,10 +920,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9F4730-5ACD-4706-939C-D5C08F6F4079}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,13 +940,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -890,7 +1004,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -901,7 +1015,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -956,7 +1070,7 @@
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12" t="s">
         <v>49</v>
@@ -978,7 +1092,7 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" t="s">
         <v>51</v>
@@ -992,7 +1106,7 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1000,7 +1114,7 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
         <v>54</v>
@@ -1180,7 +1294,7 @@
         <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" t="s">
         <v>84</v>
@@ -1212,7 +1326,227 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>129</v>
+      </c>
+      <c r="B50" t="s">
+        <v>130</v>
+      </c>
+      <c r="D50" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1247,10 +1581,11 @@
     <hyperlink ref="A12" r:id="rId29" xr:uid="{8F60D9F8-D490-483F-AF2F-8A8B9EED2252}"/>
     <hyperlink ref="A14" r:id="rId30" xr:uid="{9A9C08B1-5EC6-4EC9-8442-FCFE7F012F47}"/>
     <hyperlink ref="A16" r:id="rId31" xr:uid="{EE40A947-8C86-4076-8EB5-285BEE3AAFD5}"/>
+    <hyperlink ref="A35" r:id="rId32" xr:uid="{58188EDC-E7D8-46A3-88A8-27503C61342B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId33"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Manual_Topic_Evaluation.xlsx should assist evaluation of discovered topics for CS 410 projects. File contains: * Discovered topics and tags, from Suhas' AlgOutput.tsv   * Plus human interpretation of those topics + tags * A couple of matching CS 410 projects per topic, from AlgOutput.tsv   * Ground truth labels for each project   * Best matching tags for the project from the topic   * A place to rate the topic's relevance to the project
Updated original Ground_Truth_Topics.xlsx to include the CS 410 projects
used in Manual_Topic_Evaluation.xlsx.
</commit_message>
<xml_diff>
--- a/topic-files/Ground_Truth_Topics.xlsx
+++ b/topic-files/Ground_Truth_Topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktuoh\Documents\School\MCS-DS\CS_410_Text_Info_Systems\Project\CourseProject\topic-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C633D58-7D1A-4A0F-A951-483CD68C8B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E12F3E9-7A3B-415F-94CF-AE83F9688581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19370" yWindow="3670" windowWidth="23600" windowHeight="18160" activeTab="1" xr2:uid="{0F37B134-5501-4313-8724-3C793E42205F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="149">
   <si>
     <t>Project Link</t>
   </si>
@@ -468,6 +468,21 @@
   </si>
   <si>
     <t>Analyze stock sentiment from Twitter</t>
+  </si>
+  <si>
+    <t>https://github.com/sjma3/CourseProject</t>
+  </si>
+  <si>
+    <t>Add autoscrolling functionality</t>
+  </si>
+  <si>
+    <t>https://github.com/ss129/CourseProject</t>
+  </si>
+  <si>
+    <t>https://github.com/subhasishb-coder/CourseProject</t>
+  </si>
+  <si>
+    <t>https://github.com/Ehaly/CourseProject</t>
   </si>
 </sst>
 </file>
@@ -563,8 +578,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{211A4259-A08B-4C0C-A237-5C41C49A6EC2}" name="Selected_Project_Topic_Table4" displayName="Selected_Project_Topic_Table4" ref="A1:E43" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E43" xr:uid="{612C9047-1189-4A6B-B897-EB8BF18B9FF9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{211A4259-A08B-4C0C-A237-5C41C49A6EC2}" name="Selected_Project_Topic_Table4" displayName="Selected_Project_Topic_Table4" ref="A1:E44" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E44" xr:uid="{612C9047-1189-4A6B-B897-EB8BF18B9FF9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{6A14DB56-DD12-401C-9F31-AB678A85BC28}" name="Project Link"/>
     <tableColumn id="2" xr3:uid="{67882653-FA50-478E-913F-6E9070B41516}" name="High-Level Topic"/>
@@ -920,15 +935,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9F4730-5ACD-4706-939C-D5C08F6F4079}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.5703125" customWidth="1"/>
     <col min="2" max="2" width="39.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="66.42578125" customWidth="1"/>
@@ -1338,214 +1351,297 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>38</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>107</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" t="s">
         <v>110</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>11</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>11</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>117</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>110</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>38</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>81</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>74</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>19</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>130</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>8</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D54" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>136</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>11</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>8</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" t="s">
+        <v>41</v>
+      </c>
+      <c r="D63" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1581,11 +1677,39 @@
     <hyperlink ref="A12" r:id="rId29" xr:uid="{8F60D9F8-D490-483F-AF2F-8A8B9EED2252}"/>
     <hyperlink ref="A14" r:id="rId30" xr:uid="{9A9C08B1-5EC6-4EC9-8442-FCFE7F012F47}"/>
     <hyperlink ref="A16" r:id="rId31" xr:uid="{EE40A947-8C86-4076-8EB5-285BEE3AAFD5}"/>
-    <hyperlink ref="A35" r:id="rId32" xr:uid="{58188EDC-E7D8-46A3-88A8-27503C61342B}"/>
+    <hyperlink ref="A36" r:id="rId32" xr:uid="{58188EDC-E7D8-46A3-88A8-27503C61342B}"/>
+    <hyperlink ref="A38" r:id="rId33" xr:uid="{42D8B548-BFDB-44A1-AB91-8E6574E11C39}"/>
+    <hyperlink ref="A41" r:id="rId34" xr:uid="{64D72980-DD90-427A-933C-E8C3E8A31166}"/>
+    <hyperlink ref="A42" r:id="rId35" xr:uid="{EF10FDDF-FDCE-443C-ACB1-ABCE704CB7CD}"/>
+    <hyperlink ref="A43" r:id="rId36" xr:uid="{1EBE31A6-DA5D-48FE-BB9F-C293C7C53E3D}"/>
+    <hyperlink ref="A45" r:id="rId37" xr:uid="{6A485AFA-B507-4985-9C49-6E6B59130E96}"/>
+    <hyperlink ref="A47" r:id="rId38" xr:uid="{C8108C20-FF5D-49E3-B635-DFB376B23A2D}"/>
+    <hyperlink ref="A49" r:id="rId39" xr:uid="{95D61579-A0C8-420B-B572-9472A28250D5}"/>
+    <hyperlink ref="A51" r:id="rId40" xr:uid="{062C8EA7-A815-4C78-AF3A-C2DD3037CCAC}"/>
+    <hyperlink ref="A53" r:id="rId41" xr:uid="{AB9A5E90-68B7-41C2-A97C-7C1F481F82CB}"/>
+    <hyperlink ref="A55" r:id="rId42" xr:uid="{A8E8BFBA-D2D8-4D60-95E3-5B660473F414}"/>
+    <hyperlink ref="A57" r:id="rId43" xr:uid="{2C537C9F-2C6A-48DA-8C29-6C21B7E54945}"/>
+    <hyperlink ref="A60" r:id="rId44" xr:uid="{589FBBF5-22AA-4B8C-A1A9-0B54344483E3}"/>
+    <hyperlink ref="A61" r:id="rId45" xr:uid="{F15E43F6-F33A-4CC0-95C6-B69008456F84}"/>
+    <hyperlink ref="A62" r:id="rId46" xr:uid="{DCDEBDF2-71CD-43AC-8C76-9B7F3843037C}"/>
+    <hyperlink ref="A63" r:id="rId47" xr:uid="{E5D58E84-397C-4039-B039-2E8343A9296E}"/>
+    <hyperlink ref="A35" r:id="rId48" xr:uid="{093A9BAC-9456-4A19-84E0-6D9BC8F88F57}"/>
+    <hyperlink ref="A39" r:id="rId49" xr:uid="{3DB1486E-9E5E-4100-B6FF-92C8F046CF87}"/>
+    <hyperlink ref="A40" r:id="rId50" xr:uid="{04EC703A-E268-4B4C-BDC3-2417ECAD5147}"/>
+    <hyperlink ref="A37" r:id="rId51" xr:uid="{E18874B7-0631-48A4-8869-92E53F275EA1}"/>
+    <hyperlink ref="A44" r:id="rId52" xr:uid="{5567EED1-F0F0-4D13-828C-B3F6E2D6037E}"/>
+    <hyperlink ref="A46" r:id="rId53" xr:uid="{24B02C5E-87C7-448D-9D8B-51916568151D}"/>
+    <hyperlink ref="A48" r:id="rId54" xr:uid="{06DA28C9-A7FC-45E7-9CE4-DAD4EE04ED1A}"/>
+    <hyperlink ref="A50" r:id="rId55" xr:uid="{0FFAA3E2-E8D5-4F1B-9FEA-7FF09B18E53B}"/>
+    <hyperlink ref="A52" r:id="rId56" xr:uid="{667F3531-7D9A-4AD5-9A47-8DEF92BC8019}"/>
+    <hyperlink ref="A54" r:id="rId57" xr:uid="{5CBDE230-182D-439E-B8B6-5676F260D613}"/>
+    <hyperlink ref="A56" r:id="rId58" xr:uid="{CDBC914C-C3F1-43F2-915E-CCF1E0707401}"/>
+    <hyperlink ref="A58" r:id="rId59" xr:uid="{0E026AA1-0EA1-495C-BB82-15FF119DF333}"/>
+    <hyperlink ref="A59" r:id="rId60" xr:uid="{1B5283CC-67F6-4DA4-9556-F3187CB94EB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId33"/>
+    <tablePart r:id="rId61"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>